<commit_message>
Actualización Arka Enero 21
</commit_message>
<xml_diff>
--- a/blocks/inventarios/asignarInventarioC/gestionContratistas/plantilla/archivo_contratista.xlsx
+++ b/blocks/inventarios/asignarInventarioC/gestionContratistas/plantilla/archivo_contratista.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="504" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="504" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datos a Cargar" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,11 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Vigencia</t>
   </si>
   <si>
+    <t>Tipo Contrato</t>
+  </si>
+  <si>
     <t>Número Contrato</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
     <t>Día Fecha Final Contrato</t>
   </si>
   <si>
+    <t>Tipo de Contrato</t>
+  </si>
+  <si>
     <t>MICHAEL STIV</t>
   </si>
   <si>
@@ -67,6 +73,15 @@
   </si>
   <si>
     <t>TINJACA</t>
+  </si>
+  <si>
+    <t>TIPO DE CONTRATO</t>
+  </si>
+  <si>
+    <t>1  : Orden de Prestación de Servicios</t>
+  </si>
+  <si>
+    <t>2  : Contrato de Prestación Servicios</t>
   </si>
 </sst>
 </file>
@@ -76,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,8 +120,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +140,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF003300"/>
         <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -154,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -165,6 +194,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -184,28 +221,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.7755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.1530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="32.3724489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.7295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.7755102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.9387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.8316326530612"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="22.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.8724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.7755102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.1530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="32.3724489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.7755102040816"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.9387755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.8316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="22.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,6 +278,9 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -259,28 +299,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6785714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9438775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.4897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.8316326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9438775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.7295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.4897959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.9387755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.8316326530612"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="22.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,7 +329,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -317,183 +358,224 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>2014</v>
-      </c>
-      <c r="B2" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>1026276984</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>2014</v>
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>12</v>
+        <v>2015</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>12</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>2015</v>
+        <v>12</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>1</v>
+        <v>2016</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1026276984</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1026276984</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="H3" s="0" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>2015</v>
+        <v>12</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>3</v>
+        <v>2016</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>2013</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>441</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>1237651763</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>2013</v>
+        <v>15</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>10</v>
+        <v>2015</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>2014</v>
+        <v>12</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>1</v>
+        <v>2016</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1237651763</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>223</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1237651763</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="H5" s="0" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>2015</v>
+        <v>12</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>10</v>
+        <v>2016</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5535353533</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>5535353533</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="H6" s="0" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>2015</v>
+        <v>12</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>10</v>
+        <v>2016</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>